<commit_message>
CargaDV- 5 DE MAYO
</commit_message>
<xml_diff>
--- a/Correos/Bot2025.xlsx
+++ b/Correos/Bot2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maaji-my.sharepoint.com/personal/pdesarrollo2_maaji_co/Documents/Escritorio/MaajiTelegrambot2025/Correos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="11_2B59D2BFD3C0D719673A221159BC40376E87EB8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6501039D-0F4F-4168-86A4-916CBFFC1EF0}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="11_2B59D2BFD3C0D719673A221159BC40376E87EB8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C60201A9-EB22-4975-B4A1-57EA0C3C3396}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -176,13 +176,22 @@
   </si>
   <si>
     <t>dgarcia@maaji.co</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>normal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +223,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -223,7 +240,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -246,11 +263,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -262,8 +291,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A17"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +619,7 @@
     <col min="5" max="5" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -599,8 +635,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -616,8 +655,11 @@
       <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -633,8 +675,11 @@
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -644,14 +689,17 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -667,8 +715,11 @@
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -684,8 +735,11 @@
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -701,8 +755,11 @@
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -718,8 +775,11 @@
       <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -735,8 +795,11 @@
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -752,8 +815,11 @@
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -769,8 +835,11 @@
       <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -786,8 +855,11 @@
       <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -803,8 +875,11 @@
       <c r="E13" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -820,8 +895,11 @@
       <c r="E14" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -835,8 +913,11 @@
         <v>49</v>
       </c>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -852,8 +933,11 @@
       <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -869,9 +953,15 @@
       <c r="E17" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="F17" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{F4B9ACF1-D1ED-40C6-A99C-621652C31BA0}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>